<commit_message>
MH45 profile for root profile
</commit_message>
<xml_diff>
--- a/payload/profile data/profiles.xlsx
+++ b/payload/profile data/profiles.xlsx
@@ -5,17 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/profile data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="24940" windowHeight="15540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="24940" windowHeight="15540" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Initial MH-61" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="centre_profile.txt" sheetId="3" r:id="rId3"/>
     <sheet name="profile_35mm_away" sheetId="4" r:id="rId4"/>
+    <sheet name="MH-45 reflex 3" sheetId="5" r:id="rId5"/>
+    <sheet name="MH45 rootprofile" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="mh61_" localSheetId="0">'Initial MH-61'!$A$1:$C$68</definedName>
@@ -37,7 +39,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="mh61" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/profile data/mh61.txt" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/profile data/mh61.txt" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -46,7 +48,7 @@
     </textPr>
   </connection>
   <connection id="2" name="mh611" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/profile data/mh61.txt" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/profile data/mh61.txt" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -55,7 +57,7 @@
     </textPr>
   </connection>
   <connection id="3" name="mh612" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/profile data/mh61.txt" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="/Users/sorinalupu/Rocket Competition/Git/RORO/payload/profile data/mh61.txt" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -64,10 +66,6 @@
     </textPr>
   </connection>
 </connections>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -158,11 +156,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mh61_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mh61" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mh61" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mh61_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4225,7 +4223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -4982,4 +4980,2377 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A61" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>0.99948999999999999</v>
+      </c>
+      <c r="B1" s="1">
+        <v>5.2199999999999998E-3</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f>100*A1</f>
+        <v>99.948999999999998</v>
+      </c>
+      <c r="F1">
+        <f>B1*100</f>
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0.99619000000000002</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4.9800000000000001E-3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E65" si="0">100*A2</f>
+        <v>99.619</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F65" si="1">B2*100</f>
+        <v>0.498</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0.98619999999999997</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4.47E-3</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>98.61999999999999</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>0.96963999999999995</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.1599999999999996E-3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>96.963999999999999</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>0.94694</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>94.694000000000003</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.44</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>0.91856000000000004</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5.3299999999999997E-3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>91.856000000000009</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.53299999999999992</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>0.90105000000000002</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6.2300000000000003E-3</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>90.105000000000004</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.623</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>0.88578000000000001</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.8300000000000002E-3</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>88.578000000000003</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>0.84779000000000004</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.247E-2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>84.779000000000011</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.2470000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>0.80595000000000006</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.8329999999999999E-2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>80.594999999999999</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>1.833</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>0.76114000000000004</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.5270000000000001E-2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>76.114000000000004</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>2.5270000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>0.71411999999999998</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3.2890000000000003E-2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>71.411999999999992</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>3.2890000000000001</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>0.66556000000000004</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.0779999999999997E-2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>66.555999999999997</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>4.0779999999999994</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>0.61597999999999997</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>61.597999999999999</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>4.8500000000000005</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>0.56579999999999997</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5.5660000000000001E-2</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>56.58</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>5.5659999999999998</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>0.51544999999999996</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6.2010000000000003E-2</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>51.544999999999995</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>6.2010000000000005</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>0.46529999999999999</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.7360000000000003E-2</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>46.53</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>6.7360000000000007</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>0.41578999999999999</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7.1609999999999993E-2</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>41.579000000000001</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>7.1609999999999996</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>0.36737999999999998</v>
+      </c>
+      <c r="B19" s="1">
+        <v>7.467E-2</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>36.738</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>7.4669999999999996</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>0.32055</v>
+      </c>
+      <c r="B20" s="1">
+        <v>7.6450000000000004E-2</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>32.055</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>7.6450000000000005</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>0.27575</v>
+      </c>
+      <c r="B21" s="1">
+        <v>7.6859999999999998E-2</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>27.574999999999999</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>7.6859999999999999</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>0.23336000000000001</v>
+      </c>
+      <c r="B22" s="1">
+        <v>7.5829999999999995E-2</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>23.336000000000002</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>7.5829999999999993</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>0.19370999999999999</v>
+      </c>
+      <c r="B23" s="1">
+        <v>7.3330000000000006E-2</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>19.370999999999999</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>7.3330000000000002</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>0.15709000000000001</v>
+      </c>
+      <c r="B24" s="1">
+        <v>6.9400000000000003E-2</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>15.709000000000001</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>6.94</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>0.12381</v>
+      </c>
+      <c r="B25" s="1">
+        <v>6.4149999999999999E-2</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>12.381</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>6.415</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>9.4140000000000001E-2</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5.7709999999999997E-2</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>9.4139999999999997</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>5.7709999999999999</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>6.8309999999999996E-2</v>
+      </c>
+      <c r="B27" s="1">
+        <v>5.0229999999999997E-2</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>6.8309999999999995</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>5.0229999999999997</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>4.6519999999999999E-2</v>
+      </c>
+      <c r="B28" s="1">
+        <v>4.1880000000000001E-2</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>4.6520000000000001</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>4.1879999999999997</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>2.8850000000000001E-2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>3.2840000000000001E-2</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>2.8850000000000002</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>3.2840000000000003</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>1.537E-2</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2.334E-2</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1.5369999999999999</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>6.0499999999999998E-3</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.3820000000000001E-2</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>1.3820000000000001</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>1.24E-3</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4.3499999999999997E-3</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f>100*A32</f>
+        <v>0.124</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.43499999999999994</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>4.4000000000000002E-4</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.66E-3</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1.1E-4</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-4.0000000000000003E-5</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>-0.06</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>7.2999999999999996E-4</v>
+      </c>
+      <c r="B37" s="1">
+        <v>-1.92E-3</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>-0.192</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>1.58E-3</v>
+      </c>
+      <c r="B38" s="1">
+        <v>-3.6700000000000001E-3</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0.158</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>-0.36699999999999999</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>3.3300000000000001E-3</v>
+      </c>
+      <c r="B39" s="1">
+        <v>-6.1399999999999996E-3</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>-0.61399999999999999</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>5.5799999999999999E-3</v>
+      </c>
+      <c r="B40" s="1">
+        <v>-8.2500000000000004E-3</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>0.55799999999999994</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>-0.82500000000000007</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>1.7729999999999999E-2</v>
+      </c>
+      <c r="B41" s="1">
+        <v>-1.545E-2</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>1.7729999999999999</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>-1.5449999999999999</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>3.4130000000000001E-2</v>
+      </c>
+      <c r="B42" s="1">
+        <v>-2.1899999999999999E-2</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>3.4130000000000003</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>-2.19</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>5.5230000000000001E-2</v>
+      </c>
+      <c r="B43" s="1">
+        <v>-2.784E-2</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>5.5229999999999997</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>-2.7839999999999998</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>8.0769999999999995E-2</v>
+      </c>
+      <c r="B44" s="1">
+        <v>-3.3029999999999997E-2</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>8.077</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>-3.3029999999999995</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>0.11056000000000001</v>
+      </c>
+      <c r="B45" s="1">
+        <v>-3.7159999999999999E-2</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>11.056000000000001</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>-3.7159999999999997</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>0.14452000000000001</v>
+      </c>
+      <c r="B46" s="1">
+        <v>-4.018E-2</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>14.452000000000002</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>-4.0179999999999998</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>0.18243000000000001</v>
+      </c>
+      <c r="B47" s="1">
+        <v>-4.2139999999999997E-2</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>18.243000000000002</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>-4.2139999999999995</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>0.224</v>
+      </c>
+      <c r="B48" s="1">
+        <v>-4.3119999999999999E-2</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>22.400000000000002</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>-4.3120000000000003</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>0.26883000000000001</v>
+      </c>
+      <c r="B49" s="1">
+        <v>-4.3189999999999999E-2</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <f>100*A49</f>
+        <v>26.883000000000003</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>-4.319</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>0.31646000000000002</v>
+      </c>
+      <c r="B50" s="1">
+        <v>-4.2419999999999999E-2</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>31.646000000000001</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>-4.242</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>0.36638999999999999</v>
+      </c>
+      <c r="B51" s="1">
+        <v>-4.0890000000000003E-2</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>36.638999999999996</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>-4.0890000000000004</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>0.41809000000000002</v>
+      </c>
+      <c r="B52" s="1">
+        <v>-3.8699999999999998E-2</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>41.809000000000005</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>-3.8699999999999997</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>0.47098000000000001</v>
+      </c>
+      <c r="B53" s="1">
+        <v>-3.6020000000000003E-2</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>47.097999999999999</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>-3.6020000000000003</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>0.52442999999999995</v>
+      </c>
+      <c r="B54" s="1">
+        <v>-3.295E-2</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>52.442999999999998</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>-3.2949999999999999</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>0.57779999999999998</v>
+      </c>
+      <c r="B55" s="1">
+        <v>-2.9610000000000001E-2</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>57.78</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>-2.9610000000000003</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>0.63044</v>
+      </c>
+      <c r="B56" s="1">
+        <v>-2.6100000000000002E-2</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>63.043999999999997</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>-2.6100000000000003</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>0.68169000000000002</v>
+      </c>
+      <c r="B57" s="1">
+        <v>-2.2530000000000001E-2</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>68.168999999999997</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>-2.2530000000000001</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>0.73090999999999995</v>
+      </c>
+      <c r="B58" s="1">
+        <v>-1.9009999999999999E-2</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>73.090999999999994</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>-1.9009999999999998</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="B59" s="1">
+        <v>-1.5650000000000001E-2</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>77.75</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>-1.5650000000000002</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>0.82089999999999996</v>
+      </c>
+      <c r="B60" s="1">
+        <v>-1.255E-2</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>82.09</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>-1.2550000000000001</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>0.86058999999999997</v>
+      </c>
+      <c r="B61" s="1">
+        <v>-9.8200000000000006E-3</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>86.058999999999997</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>-0.9820000000000001</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>0.89605000000000001</v>
+      </c>
+      <c r="B62" s="1">
+        <v>-7.4700000000000001E-3</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="0"/>
+        <v>89.605000000000004</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>-0.747</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B63" s="1">
+        <v>-7.2100000000000003E-3</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>-0.72099999999999997</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>0.90302000000000004</v>
+      </c>
+      <c r="B64" s="1">
+        <v>-6.8599999999999998E-3</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>90.302000000000007</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>-0.68599999999999994</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>0.91191999999999995</v>
+      </c>
+      <c r="B65" s="1">
+        <v>-5.8199999999999997E-3</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="0"/>
+        <v>91.191999999999993</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>-0.58199999999999996</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>0.92671000000000003</v>
+      </c>
+      <c r="B66" s="1">
+        <v>-4.0800000000000003E-3</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <f t="shared" ref="E66:E68" si="2">100*A66</f>
+        <v>92.671000000000006</v>
+      </c>
+      <c r="F66">
+        <f t="shared" ref="F66:F71" si="3">B66*100</f>
+        <v>-0.40800000000000003</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>0.95232000000000006</v>
+      </c>
+      <c r="B67" s="1">
+        <v>-1.06E-3</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="2"/>
+        <v>95.231999999999999</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="3"/>
+        <v>-0.106</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>0.97257000000000005</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1.39E-3</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="2"/>
+        <v>97.257000000000005</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>0.13899999999999998</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>0.98726000000000003</v>
+      </c>
+      <c r="B69" s="1">
+        <v>3.3600000000000001E-3</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <f>100*A69</f>
+        <v>98.725999999999999</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="3"/>
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>0.99634</v>
+      </c>
+      <c r="B70" s="1">
+        <v>4.7400000000000003E-3</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <f t="shared" ref="E70:E71" si="4">100*A70</f>
+        <v>99.634</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="3"/>
+        <v>0.47400000000000003</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>0.99948999999999999</v>
+      </c>
+      <c r="B71" s="1">
+        <v>5.2199999999999998E-3</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="4"/>
+        <v>99.948999999999998</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="3"/>
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>99.948999999999998</v>
+      </c>
+      <c r="B1">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>99.619</v>
+      </c>
+      <c r="B2">
+        <v>0.498</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>98.61999999999999</v>
+      </c>
+      <c r="B3">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>96.963999999999999</v>
+      </c>
+      <c r="B4">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>94.694000000000003</v>
+      </c>
+      <c r="B5">
+        <v>0.44</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>91.856000000000009</v>
+      </c>
+      <c r="B6">
+        <v>0.53299999999999992</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>90.105000000000004</v>
+      </c>
+      <c r="B7">
+        <v>0.623</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>88.578000000000003</v>
+      </c>
+      <c r="B8">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>84.779000000000011</v>
+      </c>
+      <c r="B9">
+        <v>1.2470000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>80.594999999999999</v>
+      </c>
+      <c r="B10">
+        <v>1.833</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>76.114000000000004</v>
+      </c>
+      <c r="B11">
+        <v>2.5270000000000001</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>71.411999999999992</v>
+      </c>
+      <c r="B12">
+        <v>3.2890000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>66.555999999999997</v>
+      </c>
+      <c r="B13">
+        <v>4.0779999999999994</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>61.597999999999999</v>
+      </c>
+      <c r="B14">
+        <v>4.8500000000000005</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>56.58</v>
+      </c>
+      <c r="B15">
+        <v>5.5659999999999998</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>51.544999999999995</v>
+      </c>
+      <c r="B16">
+        <v>6.2010000000000005</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>46.53</v>
+      </c>
+      <c r="B17">
+        <v>6.7360000000000007</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>41.579000000000001</v>
+      </c>
+      <c r="B18">
+        <v>7.1609999999999996</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>36.738</v>
+      </c>
+      <c r="B19">
+        <v>7.4669999999999996</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>32.055</v>
+      </c>
+      <c r="B20">
+        <v>7.6450000000000005</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>27.574999999999999</v>
+      </c>
+      <c r="B21">
+        <v>7.6859999999999999</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>23.336000000000002</v>
+      </c>
+      <c r="B22">
+        <v>7.5829999999999993</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19.370999999999999</v>
+      </c>
+      <c r="B23">
+        <v>7.3330000000000002</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>15.709000000000001</v>
+      </c>
+      <c r="B24">
+        <v>6.94</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>12.381</v>
+      </c>
+      <c r="B25">
+        <v>6.415</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>9.4139999999999997</v>
+      </c>
+      <c r="B26">
+        <v>5.7709999999999999</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>6.8309999999999995</v>
+      </c>
+      <c r="B27">
+        <v>5.0229999999999997</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>4.6520000000000001</v>
+      </c>
+      <c r="B28">
+        <v>4.1879999999999997</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2.8850000000000002</v>
+      </c>
+      <c r="B29">
+        <v>3.2840000000000003</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1.5369999999999999</v>
+      </c>
+      <c r="B30">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="B31">
+        <v>1.3820000000000001</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0.124</v>
+      </c>
+      <c r="B32">
+        <v>0.43499999999999994</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="B33">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="B34">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>0.02</v>
+      </c>
+      <c r="B36">
+        <v>-0.06</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="B37">
+        <v>-0.192</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0.158</v>
+      </c>
+      <c r="B38">
+        <v>-0.36699999999999999</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="B39">
+        <v>-0.61399999999999999</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>0.55799999999999994</v>
+      </c>
+      <c r="B40">
+        <v>-0.82500000000000007</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1.7729999999999999</v>
+      </c>
+      <c r="B41">
+        <v>-1.5449999999999999</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>3.4130000000000003</v>
+      </c>
+      <c r="B42">
+        <v>-2.19</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5.5229999999999997</v>
+      </c>
+      <c r="B43">
+        <v>-2.7839999999999998</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>8.077</v>
+      </c>
+      <c r="B44">
+        <v>-3.3029999999999995</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>11.056000000000001</v>
+      </c>
+      <c r="B45">
+        <v>-3.7159999999999997</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>14.452000000000002</v>
+      </c>
+      <c r="B46">
+        <v>-4.0179999999999998</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>18.243000000000002</v>
+      </c>
+      <c r="B47">
+        <v>-4.2139999999999995</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="B48">
+        <v>-4.3120000000000003</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>26.883000000000003</v>
+      </c>
+      <c r="B49">
+        <v>-4.319</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>31.646000000000001</v>
+      </c>
+      <c r="B50">
+        <v>-4.242</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>36.638999999999996</v>
+      </c>
+      <c r="B51">
+        <v>-4.0890000000000004</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>41.809000000000005</v>
+      </c>
+      <c r="B52">
+        <v>-3.8699999999999997</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>47.097999999999999</v>
+      </c>
+      <c r="B53">
+        <v>-3.6020000000000003</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>52.442999999999998</v>
+      </c>
+      <c r="B54">
+        <v>-3.2949999999999999</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>57.78</v>
+      </c>
+      <c r="B55">
+        <v>-2.9610000000000003</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>63.043999999999997</v>
+      </c>
+      <c r="B56">
+        <v>-2.6100000000000003</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>68.168999999999997</v>
+      </c>
+      <c r="B57">
+        <v>-2.2530000000000001</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>73.090999999999994</v>
+      </c>
+      <c r="B58">
+        <v>-1.9009999999999998</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>77.75</v>
+      </c>
+      <c r="B59">
+        <v>-1.5650000000000002</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>82.09</v>
+      </c>
+      <c r="B60">
+        <v>-1.2550000000000001</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>86.058999999999997</v>
+      </c>
+      <c r="B61">
+        <v>-0.9820000000000001</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>89.605000000000004</v>
+      </c>
+      <c r="B62">
+        <v>-0.747</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>90</v>
+      </c>
+      <c r="B63">
+        <v>-0.72099999999999997</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>90.302000000000007</v>
+      </c>
+      <c r="B64">
+        <v>-0.68599999999999994</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>91.191999999999993</v>
+      </c>
+      <c r="B65">
+        <v>-0.58199999999999996</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>92.671000000000006</v>
+      </c>
+      <c r="B66">
+        <v>-0.40800000000000003</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>95.231999999999999</v>
+      </c>
+      <c r="B67">
+        <v>-0.106</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>97.257000000000005</v>
+      </c>
+      <c r="B68">
+        <v>0.13899999999999998</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>98.725999999999999</v>
+      </c>
+      <c r="B69">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>99.634</v>
+      </c>
+      <c r="B70">
+        <v>0.47400000000000003</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>99.948999999999998</v>
+      </c>
+      <c r="B71">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>